<commit_message>
#713 Bypass Draft+Approval when creating new Product (-Model) and mark them with a Category
</commit_message>
<xml_diff>
--- a/pim/src/PcmtCustomDatasetBundle/Resources/fixtures/pcmt_global/import_files/2020-07-08/1_categories.xlsx
+++ b/pim/src/PcmtCustomDatasetBundle/Resources/fixtures/pcmt_global/import_files/2020-07-08/1_categories.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="890">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="893">
   <si>
     <t xml:space="preserve">code</t>
   </si>
@@ -2690,6 +2690,15 @@
   </si>
   <si>
     <t xml:space="preserve">FR High-throughput PCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEW_SKIPPED_DRAFTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Skipped Drafts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR New Skipped Drafts</t>
   </si>
 </sst>
 </file>
@@ -2765,13 +2774,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2787,7 +2800,92 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{B0810010-7A7F-0000-2100-000000000000}"/>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{5A3C6DEB-9120-4CBB-A2E9-BF57B0CA6A26}">
+  <header guid="{17BDDE48-3CF0-4A9A-8F96-70A898F187B9}" dateTime="2020-11-19T12:28:00.000000000Z" userName=" " r:id="rId1" minRId="1" maxRId="1" maxSheetId="2">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{5A3C6DEB-9120-4CBB-A2E9-BF57B0CA6A26}" dateTime="2020-11-19T12:29:00.000000000Z" userName=" " r:id="rId2" minRId="2" maxRId="4" maxSheetId="2">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+</headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="1" ua="false" sId="1">
+    <nc r="A449" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">NEW_SKIPPED_DRAFTS</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="2" ua="false" sId="1">
+    <nc r="B449" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">New Skipped Drafts</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="3" ua="false" sId="1">
+    <nc r="C449" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">FR New Skipped Drafts</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="4" ua="false" sId="1">
+    <nc r="D449" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">master</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2799,19 +2897,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D448"/>
+  <dimension ref="A1:D449"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A417" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A425" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C448" activeCellId="0" sqref="C448"/>
+      <selection pane="bottomLeft" activeCell="B454" activeCellId="0" sqref="B454"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.7111111111111"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.1888888888889"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.3518518518519"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.8666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.3"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4444444444444"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.9185185185185"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.44814814814815"/>
   </cols>
@@ -7772,6 +7870,20 @@
       </c>
       <c r="D448" s="0" t="s">
         <v>875</v>
+      </c>
+    </row>
+    <row r="449" customFormat="false" ht="15.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A449" s="0" t="s">
+        <v>890</v>
+      </c>
+      <c r="B449" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="C449" s="0" t="s">
+        <v>892</v>
+      </c>
+      <c r="D449" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>